<commit_message>
tx-export-convert Fix sorting, commission for FX. Add DIV support
USD dividends will now add to your USD.FX amount.
</commit_message>
<xml_diff>
--- a/test/QT_Test_Export.xlsx
+++ b/test/QT_Test_Export.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TXs" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="FXTs" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="TX Errors" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="FXT Errors" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sorting" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="146">
   <si>
     <t xml:space="preserve">Transaction Date</t>
   </si>
@@ -245,6 +246,9 @@
   </si>
   <si>
     <t xml:space="preserve">DIV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.5</t>
   </si>
   <si>
     <t xml:space="preserve">Ignored actions</t>
@@ -557,10 +561,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1231,27 +1235,58 @@
       </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="D15" s="0"/>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
-      <c r="G15" s="0"/>
-      <c r="H15" s="0"/>
-      <c r="I15" s="0"/>
-      <c r="J15" s="0"/>
-      <c r="K15" s="0"/>
-      <c r="L15" s="0"/>
-      <c r="M15" s="0"/>
-      <c r="N15" s="0"/>
-      <c r="O15" s="0"/>
-      <c r="P15" s="0"/>
+      <c r="A15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>10000003</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>73</v>
@@ -1288,63 +1323,67 @@
         <v>19</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="C18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1366,15 +1405,15 @@
       <c r="K19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="N19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1387,10 +1426,10 @@
       <c r="C20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1412,12 +1451,12 @@
       <c r="L20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="O20" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1433,10 +1472,10 @@
       <c r="D21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1458,11 +1497,9 @@
       <c r="M21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="N21" s="1"/>
       <c r="O21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,10 +1518,10 @@
       <c r="E22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="H22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1507,7 +1544,7 @@
         <v>19</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1529,10 +1566,10 @@
       <c r="F23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1552,7 +1589,7 @@
         <v>19</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1577,10 +1614,10 @@
       <c r="G24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="J24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1597,7 +1634,7 @@
         <v>19</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1607,7 +1644,9 @@
       <c r="B25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="D25" s="1" t="s">
         <v>19</v>
       </c>
@@ -1623,10 +1662,10 @@
       <c r="H25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K25" s="1" t="s">
         <v>19</v>
       </c>
@@ -1640,7 +1679,50 @@
         <v>19</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1661,8 +1743,8 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="1" sqref="A18:B18 G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1721,13 +1803,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -1748,7 +1830,7 @@
         <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>23</v>
@@ -1763,19 +1845,19 @@
         <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>19</v>
@@ -1796,7 +1878,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>38</v>
@@ -1811,19 +1893,19 @@
         <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -1844,7 +1926,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>38</v>
@@ -1859,19 +1941,19 @@
         <v>33</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -1892,7 +1974,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>23</v>
@@ -1907,7 +1989,7 @@
         <v>33</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P5" s="1"/>
     </row>
@@ -1929,8 +2011,8 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="1" sqref="A18:B18 B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1994,13 +2076,13 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>19</v>
@@ -2033,7 +2115,7 @@
         <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,7 +2127,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>19</v>
@@ -2078,12 +2160,12 @@
         <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
@@ -2092,7 +2174,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>19</v>
@@ -2125,7 +2207,7 @@
         <v>33</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2136,7 +2218,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -2169,7 +2251,7 @@
         <v>33</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,10 +2262,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
@@ -2216,7 +2298,7 @@
         <v>24</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2261,7 +2343,7 @@
         <v>24</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2275,13 +2357,13 @@
         <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>21</v>
@@ -2308,7 +2390,7 @@
         <v>24</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2339,7 +2421,7 @@
         <v>51</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>19</v>
@@ -2369,7 +2451,7 @@
         <v>24</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2383,7 +2465,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>19</v>
@@ -2413,7 +2495,7 @@
         <v>24</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2427,13 +2509,13 @@
         <v>51</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>21</v>
@@ -2460,7 +2542,7 @@
         <v>24</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,13 +2556,13 @@
         <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>21</v>
@@ -2507,7 +2589,7 @@
         <v>24</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2521,7 +2603,7 @@
         <v>51</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>19</v>
@@ -2551,7 +2633,7 @@
         <v>24</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,7 +2647,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>19</v>
@@ -2595,7 +2677,7 @@
         <v>24</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,7 +2691,7 @@
         <v>51</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>19</v>
@@ -2618,7 +2700,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>19</v>
@@ -2642,7 +2724,7 @@
         <v>24</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2656,7 +2738,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>19</v>
@@ -2665,7 +2747,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>19</v>
@@ -2689,7 +2771,7 @@
         <v>24</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2703,7 +2785,7 @@
         <v>51</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>19</v>
@@ -2733,7 +2815,7 @@
         <v>24</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2747,7 +2829,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>19</v>
@@ -2777,7 +2859,7 @@
         <v>24</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2791,7 +2873,7 @@
         <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>19</v>
@@ -2806,7 +2888,7 @@
         <v>19</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>19</v>
@@ -2824,7 +2906,7 @@
         <v>24</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2838,7 +2920,7 @@
         <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>19</v>
@@ -2853,7 +2935,7 @@
         <v>19</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>19</v>
@@ -2871,7 +2953,7 @@
         <v>24</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,8 +3165,8 @@
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J22" activeCellId="1" sqref="A18:B18 J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3154,7 +3236,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>19</v>
@@ -3187,18 +3269,18 @@
         <v>24</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -3219,7 +3301,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>23</v>
@@ -3234,18 +3316,18 @@
         <v>33</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -3266,7 +3348,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>38</v>
@@ -3281,18 +3363,18 @@
         <v>33</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
@@ -3313,7 +3395,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>23</v>
@@ -3328,18 +3410,18 @@
         <v>33</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>19</v>
@@ -3360,7 +3442,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>38</v>
@@ -3375,18 +3457,18 @@
         <v>33</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>19</v>
@@ -3407,7 +3489,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>23</v>
@@ -3422,18 +3504,18 @@
         <v>33</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>19</v>
@@ -3454,7 +3536,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>23</v>
@@ -3469,18 +3551,18 @@
         <v>33</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>19</v>
@@ -3501,7 +3583,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>38</v>
@@ -3516,18 +3598,18 @@
         <v>33</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
@@ -3548,7 +3630,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>38</v>
@@ -3563,18 +3645,18 @@
         <v>33</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>19</v>
@@ -3595,7 +3677,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>23</v>
@@ -3610,18 +3692,18 @@
         <v>33</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>19</v>
@@ -3642,10 +3724,10 @@
         <v>19</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L13" s="1" t="n">
         <v>10000003</v>
@@ -3657,42 +3739,42 @@
         <v>33</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="L14" s="1" t="n">
         <v>10000003</v>
@@ -3704,18 +3786,18 @@
         <v>33</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>19</v>
@@ -3736,7 +3818,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>23</v>
@@ -3751,18 +3833,18 @@
         <v>33</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>19</v>
@@ -3783,7 +3865,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>38</v>
@@ -3798,18 +3880,18 @@
         <v>33</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
@@ -3830,10 +3912,10 @@
         <v>19</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L17" s="1" t="n">
         <v>10000003</v>
@@ -3845,18 +3927,18 @@
         <v>33</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>19</v>
@@ -3877,10 +3959,10 @@
         <v>19</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L18" s="1" t="n">
         <v>10000003</v>
@@ -3892,18 +3974,18 @@
         <v>33</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>19</v>
@@ -3924,7 +4006,7 @@
         <v>19</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>38</v>
@@ -3939,18 +4021,18 @@
         <v>33</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>19</v>
@@ -3971,10 +4053,10 @@
         <v>19</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="L20" s="1" t="n">
         <v>10000003</v>
@@ -3986,18 +4068,18 @@
         <v>33</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>19</v>
@@ -4018,10 +4100,10 @@
         <v>19</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L21" s="1" t="n">
         <v>10000003</v>
@@ -4033,18 +4115,18 @@
         <v>33</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>19</v>
@@ -4065,7 +4147,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>23</v>
@@ -4080,7 +4162,7 @@
         <v>33</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4243,4 +4325,701 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="A18:B18 A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.01"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>10000003</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>10000003</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>10000003</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>10000003</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>10000003</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>10000003</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>10000003</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>10000003</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>10000003</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
+      <c r="F15" s="0"/>
+      <c r="G15" s="0"/>
+      <c r="H15" s="0"/>
+      <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
+      <c r="L15" s="0"/>
+      <c r="M15" s="0"/>
+      <c r="N15" s="0"/>
+      <c r="O15" s="0"/>
+      <c r="P15" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add LIQ support to tx-export-convert
</commit_message>
<xml_diff>
--- a/test/QT_Test_Export.xlsx
+++ b/test/QT_Test_Export.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="151">
   <si>
     <t xml:space="preserve">Transaction Date</t>
   </si>
@@ -167,6 +167,9 @@
     <t xml:space="preserve">2023-01-15 12:00:00 AM</t>
   </si>
   <si>
+    <t xml:space="preserve">BUY</t>
+  </si>
+  <si>
     <t xml:space="preserve">-1.00</t>
   </si>
   <si>
@@ -179,21 +182,24 @@
     <t xml:space="preserve">2023-01-17 12:00:00 AM</t>
   </si>
   <si>
+    <t xml:space="preserve">SELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sell in TFSA (CAD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-01-18 12:00:00 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-01-19 12:00:00 AM</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sell</t>
   </si>
   <si>
-    <t xml:space="preserve">1.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sell in TFSA (CAD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-01-18 12:00:00 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-01-19 12:00:00 AM</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sell in RRSP (CAD)</t>
   </si>
   <si>
@@ -245,10 +251,19 @@
     <t xml:space="preserve">DIS, behaves like buy</t>
   </si>
   <si>
+    <t xml:space="preserve">LIQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIQ, behaves like sell</t>
+  </si>
+  <si>
     <t xml:space="preserve">DIV</t>
   </si>
   <si>
     <t xml:space="preserve">30.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIV, behaves like buy of USD</t>
   </si>
   <si>
     <t xml:space="preserve">Ignored actions</t>
@@ -476,6 +491,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -561,13 +577,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18:B18"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.67"/>
@@ -866,7 +882,7 @@
         <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>42</v>
@@ -884,7 +900,7 @@
         <v>19</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>19</v>
@@ -902,18 +918,18 @@
         <v>33</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>18</v>
@@ -931,7 +947,7 @@
         <v>19</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>19</v>
@@ -949,18 +965,18 @@
         <v>24</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>18</v>
@@ -978,7 +994,7 @@
         <v>19</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>19</v>
@@ -996,18 +1012,18 @@
         <v>29</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>18</v>
@@ -1025,7 +1041,7 @@
         <v>19</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>19</v>
@@ -1043,18 +1059,18 @@
         <v>33</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>42</v>
@@ -1072,7 +1088,7 @@
         <v>19</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>19</v>
@@ -1090,18 +1106,18 @@
         <v>24</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>42</v>
@@ -1119,7 +1135,7 @@
         <v>19</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>19</v>
@@ -1137,18 +1153,18 @@
         <v>29</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>42</v>
@@ -1166,7 +1182,7 @@
         <v>19</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>19</v>
@@ -1184,18 +1200,18 @@
         <v>33</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>42</v>
@@ -1231,18 +1247,18 @@
         <v>33</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>42</v>
@@ -1250,20 +1266,20 @@
       <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>19</v>
+      <c r="F15" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>38</v>
@@ -1278,63 +1294,65 @@
         <v>33</v>
       </c>
       <c r="O15" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>10000003</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>77</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>19</v>
@@ -1357,55 +1375,57 @@
       <c r="J18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="M19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1413,20 +1433,20 @@
         <v>19</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1448,15 +1468,15 @@
       <c r="K20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="N20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,12 +1487,12 @@
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1494,12 +1514,12 @@
       <c r="L21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="O21" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,15 +1530,15 @@
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1540,11 +1560,9 @@
       <c r="M22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="N22" s="1"/>
       <c r="O22" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,41 +1573,41 @@
         <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O23" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,7 +1618,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>19</v>
@@ -1611,10 +1629,10 @@
       <c r="F24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1634,7 +1652,7 @@
         <v>19</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1645,7 +1663,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>19</v>
@@ -1659,10 +1677,10 @@
       <c r="G25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="J25" s="1" t="s">
         <v>19</v>
       </c>
@@ -1679,7 +1697,7 @@
         <v>19</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,7 +1707,9 @@
       <c r="B26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="D26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1705,10 +1725,10 @@
       <c r="H26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1722,7 +1742,50 @@
         <v>19</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1744,14 +1807,14 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="1" sqref="A18:B18 G5"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,13 +1866,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -1830,7 +1893,7 @@
         <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>23</v>
@@ -1845,19 +1908,19 @@
         <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>19</v>
@@ -1878,7 +1941,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>38</v>
@@ -1893,19 +1956,19 @@
         <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -1926,7 +1989,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>38</v>
@@ -1941,19 +2004,19 @@
         <v>33</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="P4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -1974,7 +2037,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>23</v>
@@ -1989,7 +2052,7 @@
         <v>33</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="P5" s="1"/>
     </row>
@@ -2012,10 +2075,10 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="1" sqref="A18:B18 B29"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.67"/>
@@ -2076,13 +2139,13 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>19</v>
@@ -2097,7 +2160,7 @@
         <v>19</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>19</v>
@@ -2115,7 +2178,7 @@
         <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2127,7 +2190,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>19</v>
@@ -2142,7 +2205,7 @@
         <v>19</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>19</v>
@@ -2160,12 +2223,12 @@
         <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
@@ -2174,7 +2237,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>19</v>
@@ -2189,7 +2252,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>19</v>
@@ -2207,7 +2270,7 @@
         <v>33</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,7 +2281,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -2233,7 +2296,7 @@
         <v>19</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>19</v>
@@ -2251,7 +2314,7 @@
         <v>33</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2262,10 +2325,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
@@ -2298,7 +2361,7 @@
         <v>24</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2343,7 +2406,7 @@
         <v>24</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2357,13 +2420,13 @@
         <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>21</v>
@@ -2390,7 +2453,7 @@
         <v>24</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2412,16 +2475,16 @@
     </row>
     <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>19</v>
@@ -2451,21 +2514,21 @@
         <v>24</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>19</v>
@@ -2495,27 +2558,27 @@
         <v>24</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>21</v>
@@ -2542,27 +2605,27 @@
         <v>24</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>21</v>
@@ -2589,21 +2652,21 @@
         <v>24</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>19</v>
@@ -2633,21 +2696,21 @@
         <v>24</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>19</v>
@@ -2677,21 +2740,21 @@
         <v>24</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>19</v>
@@ -2700,7 +2763,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>19</v>
@@ -2724,21 +2787,21 @@
         <v>24</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>19</v>
@@ -2747,7 +2810,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>19</v>
@@ -2771,21 +2834,21 @@
         <v>24</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>19</v>
@@ -2815,21 +2878,21 @@
         <v>24</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>19</v>
@@ -2859,21 +2922,21 @@
         <v>24</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>19</v>
@@ -2888,7 +2951,7 @@
         <v>19</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>19</v>
@@ -2906,21 +2969,21 @@
         <v>24</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>19</v>
@@ -2935,7 +2998,7 @@
         <v>19</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>19</v>
@@ -2953,7 +3016,7 @@
         <v>24</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3166,10 +3229,10 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="1" sqref="A18:B18 J22"/>
+      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.67"/>
@@ -3236,7 +3299,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>19</v>
@@ -3269,18 +3332,18 @@
         <v>24</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -3301,7 +3364,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>23</v>
@@ -3316,18 +3379,18 @@
         <v>33</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -3348,7 +3411,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>38</v>
@@ -3363,18 +3426,18 @@
         <v>33</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
@@ -3395,7 +3458,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>23</v>
@@ -3410,18 +3473,18 @@
         <v>33</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>19</v>
@@ -3442,7 +3505,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>38</v>
@@ -3457,18 +3520,18 @@
         <v>33</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>19</v>
@@ -3489,7 +3552,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>23</v>
@@ -3504,18 +3567,18 @@
         <v>33</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>19</v>
@@ -3536,7 +3599,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>23</v>
@@ -3551,18 +3614,18 @@
         <v>33</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>19</v>
@@ -3583,7 +3646,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>38</v>
@@ -3598,18 +3661,18 @@
         <v>33</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
@@ -3630,7 +3693,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>38</v>
@@ -3645,18 +3708,18 @@
         <v>33</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>19</v>
@@ -3677,7 +3740,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>23</v>
@@ -3692,18 +3755,18 @@
         <v>33</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>19</v>
@@ -3724,10 +3787,10 @@
         <v>19</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="L13" s="1" t="n">
         <v>10000003</v>
@@ -3739,18 +3802,18 @@
         <v>33</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>19</v>
@@ -3771,10 +3834,10 @@
         <v>19</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="L14" s="1" t="n">
         <v>10000003</v>
@@ -3786,18 +3849,18 @@
         <v>33</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>19</v>
@@ -3818,7 +3881,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>23</v>
@@ -3833,18 +3896,18 @@
         <v>33</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>19</v>
@@ -3865,7 +3928,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>38</v>
@@ -3880,18 +3943,18 @@
         <v>33</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
@@ -3912,10 +3975,10 @@
         <v>19</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="L17" s="1" t="n">
         <v>10000003</v>
@@ -3927,42 +3990,42 @@
         <v>33</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="L18" s="1" t="n">
         <v>10000003</v>
@@ -3974,18 +4037,18 @@
         <v>33</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>19</v>
@@ -4006,7 +4069,7 @@
         <v>19</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>38</v>
@@ -4021,18 +4084,18 @@
         <v>33</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>19</v>
@@ -4053,10 +4116,10 @@
         <v>19</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="L20" s="1" t="n">
         <v>10000003</v>
@@ -4068,18 +4131,18 @@
         <v>33</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>19</v>
@@ -4100,10 +4163,10 @@
         <v>19</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="L21" s="1" t="n">
         <v>10000003</v>
@@ -4115,18 +4178,18 @@
         <v>33</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>19</v>
@@ -4147,7 +4210,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>23</v>
@@ -4162,7 +4225,7 @@
         <v>33</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4335,10 +4398,10 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="A18:B18 A16"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.67"/>
@@ -4399,10 +4462,10 @@
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -4423,7 +4486,7 @@
         <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>23</v>
@@ -4438,7 +4501,7 @@
         <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P2" s="1"/>
     </row>
@@ -4447,10 +4510,10 @@
         <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>19</v>
@@ -4471,7 +4534,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>38</v>
@@ -4486,7 +4549,7 @@
         <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P3" s="1"/>
     </row>
@@ -4495,10 +4558,10 @@
         <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -4519,7 +4582,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>38</v>
@@ -4534,7 +4597,7 @@
         <v>33</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="P4" s="1"/>
     </row>
@@ -4543,10 +4606,10 @@
         <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -4567,7 +4630,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>23</v>
@@ -4582,7 +4645,7 @@
         <v>33</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="P5" s="1"/>
     </row>
@@ -4684,7 +4747,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>42</v>
@@ -4729,7 +4792,7 @@
         <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>42</v>
@@ -4774,7 +4837,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>42</v>

</xml_diff>